<commit_message>
Implement excel bridge WIP
</commit_message>
<xml_diff>
--- a/.Dev-App/Unity/Assets/Resources/LocaDemo.xlsx
+++ b/.Dev-App/Unity/Assets/Resources/LocaDemo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Programming\unity-gui-toolkit\.Dev-App\Unity\Assets\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40001_{4D44F48E-B996-4EE5-AB41-88407657BA21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40001_{24AC7044-DF5F-4EA6-86DA-41B385628303}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6960" yWindow="3930" windowWidth="28800" windowHeight="15555"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>excel_key1</t>
   </si>
@@ -54,6 +54,12 @@
   </si>
   <si>
     <t>Excel Schlüssel 1</t>
+  </si>
+  <si>
+    <t>Bla</t>
+  </si>
+  <si>
+    <t>Blupp</t>
   </si>
 </sst>
 </file>
@@ -405,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -418,7 +424,7 @@
     <col min="3" max="3" width="22.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -428,8 +434,14 @@
       <c r="C1" t="s">
         <v>4</v>
       </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -438,6 +450,12 @@
       </c>
       <c r="C2" t="s">
         <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improved LocaExcelBridge All sheets supported
</commit_message>
<xml_diff>
--- a/.Dev-App/Unity/Assets/Resources/LocaDemo.xlsx
+++ b/.Dev-App/Unity/Assets/Resources/LocaDemo.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Programming\unity-gui-toolkit\.Dev-App\Unity\Assets\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_programming\unity-gui-toolkit\.Dev-App\Unity\Assets\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDA9E945-A0C5-49FB-8324-6CCBB4AC1512}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3AFE8CB-C249-4B40-B320-0121D2B92C55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6960" yWindow="3930" windowWidth="28800" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5070" yWindow="2205" windowWidth="28800" windowHeight="15555" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="26">
   <si>
     <t>excel_key1</t>
   </si>
@@ -93,6 +94,27 @@
   </si>
   <si>
     <t>Hunde</t>
+  </si>
+  <si>
+    <t>excel_cat</t>
+  </si>
+  <si>
+    <t>cat</t>
+  </si>
+  <si>
+    <t>Katze</t>
+  </si>
+  <si>
+    <t>Katzenbeschreibung</t>
+  </si>
+  <si>
+    <t>Noch ne Katzenbeschreibung</t>
+  </si>
+  <si>
+    <t>cats</t>
+  </si>
+  <si>
+    <t>Katzen</t>
   </si>
 </sst>
 </file>
@@ -148,9 +170,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 – 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -188,7 +210,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 – 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -294,7 +316,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 – 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -436,7 +458,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -446,8 +468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I4" sqref="A1:I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -552,4 +574,110 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E66A925-0925-48D8-9861-2008640BEC36}">
+  <dimension ref="A1:I3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="36.28515625" customWidth="1"/>
+    <col min="5" max="5" width="30.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Excel sheet can be downloaded from Google docs
</commit_message>
<xml_diff>
--- a/.Dev-App/Unity/Assets/Resources/LocaDemo.xlsx
+++ b/.Dev-App/Unity/Assets/Resources/LocaDemo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_programming\unity-gui-toolkit\.Dev-App\Unity\Assets\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3AFE8CB-C249-4B40-B320-0121D2B92C55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E9B4AEA-7BDA-4460-B291-EA90EA47D783}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5070" yWindow="2205" windowWidth="28800" windowHeight="15555" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -105,16 +105,16 @@
     <t>Katze</t>
   </si>
   <si>
-    <t>Katzenbeschreibung</t>
-  </si>
-  <si>
-    <t>Noch ne Katzenbeschreibung</t>
-  </si>
-  <si>
     <t>cats</t>
   </si>
   <si>
     <t>Katzen</t>
+  </si>
+  <si>
+    <t>Katzenbeschreibung!</t>
+  </si>
+  <si>
+    <t>Noch ne Katzenbeschreibung…</t>
   </si>
 </sst>
 </file>
@@ -581,7 +581,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -659,22 +659,22 @@
         <v>21</v>
       </c>
       <c r="D3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F3" t="s">
         <v>20</v>
       </c>
       <c r="G3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H3" t="s">
         <v>21</v>
       </c>
       <c r="I3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>